<commit_message>
Performed some more tests using different parameters. The testing files such as batch_tests_nn.py may not have everything uncommented and correct parameters.
</commit_message>
<xml_diff>
--- a/ClassifierTesterResults/Individual/OpenBCI/LR-MM-Parsed_Results.xlsx
+++ b/ClassifierTesterResults/Individual/OpenBCI/LR-MM-Parsed_Results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="228">
   <si>
     <t>subject_no</t>
   </si>
@@ -160,547 +160,544 @@
     <t>motor_cortex</t>
   </si>
   <si>
-    <t>0.40736842105263155</t>
-  </si>
-  <si>
-    <t>0.45894736842105266</t>
-  </si>
-  <si>
-    <t>0.3957894736842105</t>
-  </si>
-  <si>
-    <t>0.5531578947368421</t>
+    <t>0.45736842105263154</t>
+  </si>
+  <si>
+    <t>0.4663157894736842</t>
+  </si>
+  <si>
+    <t>0.5736842105263158</t>
+  </si>
+  <si>
+    <t>0.531578947368421</t>
+  </si>
+  <si>
+    <t>0.6131578947368421</t>
+  </si>
+  <si>
+    <t>0.5222222222222221</t>
+  </si>
+  <si>
+    <t>0.24444444444444446</t>
+  </si>
+  <si>
+    <t>0.7022222222222223</t>
+  </si>
+  <si>
+    <t>0.37555555555555553</t>
+  </si>
+  <si>
+    <t>0.6644444444444445</t>
+  </si>
+  <si>
+    <t>0.46410922410922406</t>
+  </si>
+  <si>
+    <t>0.42333333333333334</t>
+  </si>
+  <si>
+    <t>0.5535714285714286</t>
+  </si>
+  <si>
+    <t>0.545</t>
+  </si>
+  <si>
+    <t>0.6051282051282051</t>
+  </si>
+  <si>
+    <t>0.48215132693393564</t>
+  </si>
+  <si>
+    <t>0.3093406593406593</t>
+  </si>
+  <si>
+    <t>0.6105561105561106</t>
+  </si>
+  <si>
+    <t>0.4409430438842203</t>
+  </si>
+  <si>
+    <t>0.6291533180778032</t>
+  </si>
+  <si>
+    <t>0.45344444444444443</t>
+  </si>
+  <si>
+    <t>0.4315555555555556</t>
+  </si>
+  <si>
+    <t>0.635</t>
+  </si>
+  <si>
+    <t>0.46799999999999997</t>
+  </si>
+  <si>
+    <t>0.634</t>
+  </si>
+  <si>
+    <t>0.48894736842105263</t>
+  </si>
+  <si>
+    <t>0.47894736842105257</t>
   </si>
   <si>
     <t>0.625263157894737</t>
   </si>
   <si>
-    <t>0.16666666666666669</t>
-  </si>
-  <si>
-    <t>0.16888888888888887</t>
-  </si>
-  <si>
-    <t>0.06222222222222222</t>
-  </si>
-  <si>
-    <t>0.31777777777777777</t>
-  </si>
-  <si>
-    <t>0.6644444444444443</t>
-  </si>
-  <si>
-    <t>0.32666666666666666</t>
+    <t>0.48052631578947363</t>
+  </si>
+  <si>
+    <t>0.5631578947368421</t>
+  </si>
+  <si>
+    <t>0.45999999999999996</t>
   </si>
   <si>
     <t>0.4</t>
   </si>
   <si>
-    <t>0.18333333333333332</t>
-  </si>
-  <si>
-    <t>0.6085714285714285</t>
-  </si>
-  <si>
-    <t>0.6192857142857142</t>
-  </si>
-  <si>
-    <t>0.2188095238095238</t>
-  </si>
-  <si>
-    <t>0.23498168498168498</t>
-  </si>
-  <si>
-    <t>0.08993506493506494</t>
-  </si>
-  <si>
-    <t>0.40095238095238095</t>
-  </si>
-  <si>
-    <t>0.6372961816305469</t>
-  </si>
-  <si>
-    <t>0.34344444444444444</t>
-  </si>
-  <si>
-    <t>0.4348888888888888</t>
-  </si>
-  <si>
-    <t>0.29977777777777775</t>
-  </si>
-  <si>
-    <t>0.49499999999999994</t>
-  </si>
-  <si>
-    <t>0.6015555555555555</t>
+    <t>0.6866666666666665</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.6533333333333333</t>
+  </si>
+  <si>
+    <t>0.3094736842105263</t>
+  </si>
+  <si>
+    <t>0.1894736842105263</t>
+  </si>
+  <si>
+    <t>0.6176184926184927</t>
+  </si>
+  <si>
+    <t>0.4963059163059163</t>
+  </si>
+  <si>
+    <t>0.5522222222222222</t>
+  </si>
+  <si>
+    <t>0.3371428571428572</t>
+  </si>
+  <si>
+    <t>0.2571428571428572</t>
+  </si>
+  <si>
+    <t>0.644927536231884</t>
+  </si>
+  <si>
+    <t>0.4894984520123839</t>
+  </si>
+  <si>
+    <t>0.5908771929824562</t>
+  </si>
+  <si>
+    <t>0.4666666666666666</t>
+  </si>
+  <si>
+    <t>0.40822222222222226</t>
+  </si>
+  <si>
+    <t>0.6815555555555557</t>
+  </si>
+  <si>
+    <t>0.476</t>
   </si>
   <si>
     <t>0.4894736842105263</t>
   </si>
   <si>
-    <t>0.53</t>
-  </si>
-  <si>
-    <t>0.5210526315789473</t>
-  </si>
-  <si>
-    <t>0.5626315789473685</t>
-  </si>
-  <si>
-    <t>0.5747368421052632</t>
-  </si>
-  <si>
-    <t>0.4644444444444444</t>
-  </si>
-  <si>
-    <t>0.47777777777777775</t>
-  </si>
-  <si>
-    <t>0.5866666666666667</t>
-  </si>
-  <si>
-    <t>0.6288888888888888</t>
-  </si>
-  <si>
-    <t>0.5822222222222222</t>
-  </si>
-  <si>
-    <t>0.4997979797979798</t>
-  </si>
-  <si>
-    <t>0.5462337662337662</t>
-  </si>
-  <si>
-    <t>0.5291666666666666</t>
+    <t>0.4473684210526316</t>
+  </si>
+  <si>
+    <t>0.5621052631578947</t>
+  </si>
+  <si>
+    <t>0.41578947368421054</t>
+  </si>
+  <si>
+    <t>0.5842105263157895</t>
+  </si>
+  <si>
+    <t>0.48666666666666664</t>
+  </si>
+  <si>
+    <t>0.4377777777777778</t>
+  </si>
+  <si>
+    <t>0.5799999999999998</t>
+  </si>
+  <si>
+    <t>0.39555555555555555</t>
+  </si>
+  <si>
+    <t>0.5666666666666667</t>
+  </si>
+  <si>
+    <t>0.49028749028749025</t>
+  </si>
+  <si>
+    <t>0.4411111111111111</t>
+  </si>
+  <si>
+    <t>0.5646825396825397</t>
+  </si>
+  <si>
+    <t>0.4234920634920635</t>
+  </si>
+  <si>
+    <t>0.5800000000000001</t>
+  </si>
+  <si>
+    <t>0.4771903242955874</t>
+  </si>
+  <si>
+    <t>0.4374569221628045</t>
   </si>
   <si>
     <t>0.5646464646464647</t>
   </si>
   <si>
-    <t>0.5532323232323233</t>
-  </si>
-  <si>
-    <t>0.4673851294903927</t>
-  </si>
-  <si>
-    <t>0.5043785935426801</t>
-  </si>
-  <si>
-    <t>0.5462371079213184</t>
-  </si>
-  <si>
-    <t>0.5849757727652464</t>
-  </si>
-  <si>
-    <t>0.5580770107085896</t>
-  </si>
-  <si>
-    <t>0.5675555555555556</t>
-  </si>
-  <si>
-    <t>0.5155555555555555</t>
-  </si>
-  <si>
-    <t>0.5295555555555556</t>
-  </si>
-  <si>
-    <t>0.5731111111111111</t>
-  </si>
-  <si>
-    <t>0.5566666666666666</t>
-  </si>
-  <si>
-    <t>0.46842105263157896</t>
-  </si>
-  <si>
-    <t>0.38473684210526315</t>
-  </si>
-  <si>
-    <t>0.5310526315789474</t>
-  </si>
-  <si>
-    <t>0.44842105263157894</t>
-  </si>
-  <si>
-    <t>0.31555555555555553</t>
-  </si>
-  <si>
-    <t>0.3355555555555555</t>
-  </si>
-  <si>
-    <t>0.5044444444444445</t>
-  </si>
-  <si>
-    <t>0.3605555555555555</t>
-  </si>
-  <si>
-    <t>0.4523809523809524</t>
-  </si>
-  <si>
-    <t>0.3505555555555555</t>
-  </si>
-  <si>
-    <t>0.5311111111111111</t>
-  </si>
-  <si>
-    <t>0.45666666666666667</t>
-  </si>
-  <si>
-    <t>0.3307936507936508</t>
-  </si>
-  <si>
-    <t>0.3830065359477124</t>
-  </si>
-  <si>
-    <t>0.3284210526315789</t>
-  </si>
-  <si>
-    <t>0.5112236920286456</t>
-  </si>
-  <si>
-    <t>0.5081499202551835</t>
-  </si>
-  <si>
-    <t>0.37022222222222223</t>
-  </si>
-  <si>
-    <t>0.4411111111111111</t>
-  </si>
-  <si>
-    <t>0.3662222222222223</t>
-  </si>
-  <si>
-    <t>0.5515555555555556</t>
+    <t>0.4040886530050617</t>
+  </si>
+  <si>
+    <t>0.5716821465428277</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>0.3884444444444444</t>
+  </si>
+  <si>
+    <t>0.6137777777777778</t>
+  </si>
+  <si>
+    <t>0.4637777777777778</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>0.521578947368421</t>
+  </si>
+  <si>
+    <t>0.4257894736842105</t>
+  </si>
+  <si>
+    <t>0.51</t>
+  </si>
+  <si>
+    <t>0.46736842105263154</t>
+  </si>
+  <si>
+    <t>0.5742105263157895</t>
+  </si>
+  <si>
+    <t>0.5022222222222222</t>
+  </si>
+  <si>
+    <t>0.41111111111111115</t>
+  </si>
+  <si>
+    <t>0.8311111111111111</t>
+  </si>
+  <si>
+    <t>0.45555555555555555</t>
+  </si>
+  <si>
+    <t>0.691111111111111</t>
+  </si>
+  <si>
+    <t>0.5688888888888889</t>
+  </si>
+  <si>
+    <t>0.40991452991452987</t>
+  </si>
+  <si>
+    <t>0.5060474716202269</t>
+  </si>
+  <si>
+    <t>0.4731746031746032</t>
+  </si>
+  <si>
+    <t>0.5663492063492064</t>
+  </si>
+  <si>
+    <t>0.518558352402746</t>
+  </si>
+  <si>
+    <t>0.4059496567505721</t>
+  </si>
+  <si>
+    <t>0.6279278138708424</t>
+  </si>
+  <si>
+    <t>0.4590633446361001</t>
+  </si>
+  <si>
+    <t>0.6155236576289208</t>
+  </si>
+  <si>
+    <t>0.5522222222222223</t>
+  </si>
+  <si>
+    <t>0.3988888888888889</t>
+  </si>
+  <si>
+    <t>0.5137777777777777</t>
+  </si>
+  <si>
+    <t>0.45511111111111113</t>
+  </si>
+  <si>
+    <t>0.626</t>
+  </si>
+  <si>
+    <t>0.4689473684210526</t>
+  </si>
+  <si>
+    <t>0.45789473684210524</t>
+  </si>
+  <si>
+    <t>0.6242105263157895</t>
+  </si>
+  <si>
+    <t>0.4989473684210527</t>
+  </si>
+  <si>
+    <t>0.7078947368421052</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>0.4955555555555556</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>0.7333333333333333</t>
+  </si>
+  <si>
+    <t>0.27836257309941514</t>
+  </si>
+  <si>
+    <t>0.4584415584415584</t>
+  </si>
+  <si>
+    <t>0.6482251082251083</t>
+  </si>
+  <si>
+    <t>0.306140350877193</t>
+  </si>
+  <si>
+    <t>0.7044733044733045</t>
+  </si>
+  <si>
+    <t>0.3413533834586467</t>
+  </si>
+  <si>
+    <t>0.46392156862745093</t>
+  </si>
+  <si>
+    <t>0.6157575757575758</t>
+  </si>
+  <si>
+    <t>0.38441558441558443</t>
+  </si>
+  <si>
+    <t>0.711297852474323</t>
+  </si>
+  <si>
+    <t>0.5586666666666666</t>
+  </si>
+  <si>
+    <t>0.4608888888888889</t>
+  </si>
+  <si>
+    <t>0.6164444444444445</t>
+  </si>
+  <si>
+    <t>0.43933333333333335</t>
+  </si>
+  <si>
+    <t>0.7857777777777778</t>
+  </si>
+  <si>
+    <t>0.43684210526315786</t>
+  </si>
+  <si>
+    <t>0.6252631578947369</t>
+  </si>
+  <si>
+    <t>0.5066666666666666</t>
+  </si>
+  <si>
+    <t>0.4533333333333333</t>
+  </si>
+  <si>
+    <t>0.5644444444444445</t>
+  </si>
+  <si>
+    <t>0.6733333333333333</t>
+  </si>
+  <si>
+    <t>0.5045732045732045</t>
+  </si>
+  <si>
+    <t>0.4314285714285714</t>
+  </si>
+  <si>
+    <t>0.4647319347319347</t>
+  </si>
+  <si>
+    <t>0.6227777777777778</t>
+  </si>
+  <si>
+    <t>0.49630797135441096</t>
+  </si>
+  <si>
+    <t>0.4345037057885355</t>
+  </si>
+  <si>
+    <t>0.5077056277056278</t>
+  </si>
+  <si>
+    <t>0.6370760233918128</t>
+  </si>
+  <si>
+    <t>0.518</t>
+  </si>
+  <si>
+    <t>0.4642222222222222</t>
   </si>
   <si>
     <t>0.41222222222222227</t>
   </si>
   <si>
-    <t>0.4152631578947369</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>0.5205263157894737</t>
-  </si>
-  <si>
-    <t>0.5005263157894737</t>
-  </si>
-  <si>
-    <t>0.29555555555555557</t>
-  </si>
-  <si>
-    <t>0.04444444444444444</t>
-  </si>
-  <si>
-    <t>0.4022222222222222</t>
-  </si>
-  <si>
-    <t>0.7733333333333333</t>
-  </si>
-  <si>
-    <t>0.3569230769230769</t>
-  </si>
-  <si>
-    <t>0.26666666666666666</t>
+    <t>0.6955555555555556</t>
+  </si>
+  <si>
+    <t>0.5777777777777778</t>
+  </si>
+  <si>
+    <t>0.4671128871128872</t>
+  </si>
+  <si>
+    <t>0.28947368421052627</t>
+  </si>
+  <si>
+    <t>0.5236353515765281</t>
+  </si>
+  <si>
+    <t>0.3005847953216374</t>
+  </si>
+  <si>
+    <t>0.6192857142857143</t>
+  </si>
+  <si>
+    <t>0.45467914438502677</t>
+  </si>
+  <si>
+    <t>0.39047619047619053</t>
+  </si>
+  <si>
+    <t>0.5374798711755234</t>
+  </si>
+  <si>
+    <t>0.362406015037594</t>
+  </si>
+  <si>
+    <t>0.6264988558352402</t>
+  </si>
+  <si>
+    <t>0.5248888888888888</t>
+  </si>
+  <si>
+    <t>0.420888888888889</t>
+  </si>
+  <si>
+    <t>0.5539999999999999</t>
+  </si>
+  <si>
+    <t>0.45711111111111113</t>
+  </si>
+  <si>
+    <t>0.7015555555555555</t>
+  </si>
+  <si>
+    <t>0.4784210526315789</t>
+  </si>
+  <si>
+    <t>0.6036842105263158</t>
+  </si>
+  <si>
+    <t>0.5626315789473684</t>
+  </si>
+  <si>
+    <t>0.5836842105263157</t>
+  </si>
+  <si>
+    <t>0.40888888888888897</t>
   </si>
   <si>
     <t>0.44000000000000006</t>
   </si>
   <si>
-    <t>0.5533333333333333</t>
-  </si>
-  <si>
-    <t>0.5003046076730288</t>
-  </si>
-  <si>
-    <t>0.3080519480519481</t>
-  </si>
-  <si>
-    <t>0.07333333333333333</t>
-  </si>
-  <si>
-    <t>0.4264102564102564</t>
-  </si>
-  <si>
-    <t>0.41996581196581195</t>
-  </si>
-  <si>
-    <t>0.6033434970826275</t>
-  </si>
-  <si>
-    <t>0.37044444444444447</t>
-  </si>
-  <si>
-    <t>0.5213333333333334</t>
-  </si>
-  <si>
-    <t>0.46644444444444444</t>
-  </si>
-  <si>
-    <t>0.4602222222222222</t>
-  </si>
-  <si>
-    <t>0.41200000000000003</t>
-  </si>
-  <si>
-    <t>0.48894736842105263</t>
-  </si>
-  <si>
-    <t>0.5305263157894736</t>
-  </si>
-  <si>
-    <t>0.541578947368421</t>
-  </si>
-  <si>
-    <t>0.4689473684210526</t>
-  </si>
-  <si>
-    <t>0.45999999999999996</t>
-  </si>
-  <si>
-    <t>0.47555555555555545</t>
-  </si>
-  <si>
-    <t>0.5022222222222222</t>
-  </si>
-  <si>
-    <t>0.48</t>
-  </si>
-  <si>
-    <t>0.3094736842105263</t>
-  </si>
-  <si>
-    <t>0.5451082251082251</t>
-  </si>
-  <si>
-    <t>0.5139393939393939</t>
-  </si>
-  <si>
-    <t>0.5434632034632034</t>
-  </si>
-  <si>
-    <t>0.4795454545454546</t>
-  </si>
-  <si>
-    <t>0.3371428571428572</t>
-  </si>
-  <si>
-    <t>0.4956060606060606</t>
-  </si>
-  <si>
-    <t>0.503766769865841</t>
-  </si>
-  <si>
-    <t>0.5152549019607843</t>
-  </si>
-  <si>
-    <t>0.4752380952380951</t>
-  </si>
-  <si>
-    <t>0.37555555555555553</t>
-  </si>
-  <si>
-    <t>0.5328888888888889</t>
-  </si>
-  <si>
-    <t>0.49755555555555553</t>
-  </si>
-  <si>
-    <t>0.5502222222222222</t>
-  </si>
-  <si>
-    <t>0.446</t>
-  </si>
-  <si>
-    <t>0.41684210526315785</t>
-  </si>
-  <si>
-    <t>0.5105263157894736</t>
-  </si>
-  <si>
-    <t>0.4473684210526315</t>
-  </si>
-  <si>
-    <t>0.5726315789473684</t>
-  </si>
-  <si>
-    <t>0.47947368421052633</t>
-  </si>
-  <si>
-    <t>0.4355555555555556</t>
-  </si>
-  <si>
-    <t>0.4155555555555555</t>
-  </si>
-  <si>
-    <t>0.5444444444444444</t>
-  </si>
-  <si>
-    <t>0.4377777777777778</t>
-  </si>
-  <si>
-    <t>0.3156060606060606</t>
-  </si>
-  <si>
-    <t>0.5416666666666667</t>
-  </si>
-  <si>
-    <t>0.43888888888888894</t>
-  </si>
-  <si>
-    <t>0.5957575757575757</t>
-  </si>
-  <si>
-    <t>0.4953535353535353</t>
-  </si>
-  <si>
-    <t>0.3116666666666667</t>
-  </si>
-  <si>
-    <t>0.4688896707008162</t>
-  </si>
-  <si>
-    <t>0.4241235888294711</t>
-  </si>
-  <si>
-    <t>0.5628070175438598</t>
-  </si>
-  <si>
-    <t>0.45839598997493736</t>
-  </si>
-  <si>
-    <t>0.38133333333333336</t>
-  </si>
-  <si>
-    <t>0.4862222222222222</t>
-  </si>
-  <si>
-    <t>0.4086666666666667</t>
-  </si>
-  <si>
-    <t>0.4997777777777778</t>
-  </si>
-  <si>
-    <t>0.4562222222222222</t>
-  </si>
-  <si>
-    <t>0.5215789473684211</t>
-  </si>
-  <si>
-    <t>0.2733333333333333</t>
-  </si>
-  <si>
-    <t>0.42000000000000004</t>
-  </si>
-  <si>
-    <t>0.30375939849624056</t>
-  </si>
-  <si>
-    <t>0.5466666666666666</t>
-  </si>
-  <si>
-    <t>0.27836257309941514</t>
-  </si>
-  <si>
-    <t>0.3894736842105263</t>
-  </si>
-  <si>
-    <t>0.35126050420168065</t>
-  </si>
-  <si>
-    <t>0.35807692307692307</t>
-  </si>
-  <si>
-    <t>0.3413533834586467</t>
-  </si>
-  <si>
-    <t>0.29350649350649355</t>
-  </si>
-  <si>
-    <t>0.3944444444444445</t>
-  </si>
-  <si>
-    <t>0.5322222222222222</t>
-  </si>
-  <si>
-    <t>0.3702222222222222</t>
-  </si>
-  <si>
-    <t>0.3597777777777778</t>
-  </si>
-  <si>
-    <t>0.6668421052631579</t>
-  </si>
-  <si>
-    <t>0.5642105263157895</t>
-  </si>
-  <si>
-    <t>0.581578947368421</t>
-  </si>
-  <si>
-    <t>0.5221052631578947</t>
-  </si>
-  <si>
-    <t>0.6363157894736842</t>
-  </si>
-  <si>
-    <t>0.6111111111111109</t>
-  </si>
-  <si>
-    <t>0.5488888888888889</t>
-  </si>
-  <si>
-    <t>0.5822222222222223</t>
-  </si>
-  <si>
-    <t>0.6466666666666667</t>
-  </si>
-  <si>
-    <t>0.7</t>
-  </si>
-  <si>
-    <t>0.5725</t>
-  </si>
-  <si>
-    <t>0.5765234765234765</t>
-  </si>
-  <si>
-    <t>0.548611111111111</t>
-  </si>
-  <si>
-    <t>0.6306565656565656</t>
-  </si>
-  <si>
-    <t>0.6272861641282694</t>
-  </si>
-  <si>
-    <t>0.5316190476190477</t>
-  </si>
-  <si>
-    <t>0.5680570409982174</t>
-  </si>
-  <si>
-    <t>0.5171780318065148</t>
-  </si>
-  <si>
-    <t>0.6369453044375645</t>
-  </si>
-  <si>
-    <t>0.6626666666666667</t>
-  </si>
-  <si>
-    <t>0.5384444444444444</t>
-  </si>
-  <si>
-    <t>0.5795555555555556</t>
-  </si>
-  <si>
-    <t>0.5084444444444445</t>
-  </si>
-  <si>
-    <t>0.684</t>
+    <t>0.6422222222222221</t>
+  </si>
+  <si>
+    <t>0.5755555555555556</t>
+  </si>
+  <si>
+    <t>0.4802020202020202</t>
+  </si>
+  <si>
+    <t>0.5888611388611389</t>
+  </si>
+  <si>
+    <t>0.5518164188752424</t>
+  </si>
+  <si>
+    <t>0.5577777777777778</t>
+  </si>
+  <si>
+    <t>0.4190704032809295</t>
+  </si>
+  <si>
+    <t>0.31428571428571433</t>
+  </si>
+  <si>
+    <t>0.6087692056227525</t>
+  </si>
+  <si>
+    <t>0.543495514147688</t>
+  </si>
+  <si>
+    <t>0.534375712007291</t>
+  </si>
+  <si>
+    <t>0.5008888888888888</t>
+  </si>
+  <si>
+    <t>0.4928888888888888</t>
+  </si>
+  <si>
+    <t>0.6737777777777778</t>
+  </si>
+  <si>
+    <t>0.508</t>
+  </si>
+  <si>
+    <t>0.5835555555555556</t>
   </si>
 </sst>
 </file>
@@ -1233,82 +1230,82 @@
         <v>93</v>
       </c>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>97</v>
       </c>
       <c r="O2" t="s">
         <v>102</v>
       </c>
       <c r="P2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="Q2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="R2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="S2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="T2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="U2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="V2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="W2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="X2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="Y2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>182</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH2" t="s">
         <v>147</v>
       </c>
-      <c r="Z2" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>156</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>161</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>166</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>175</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>185</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>143</v>
-      </c>
       <c r="AI2" t="s">
-        <v>150</v>
+        <v>93</v>
       </c>
       <c r="AJ2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AK2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="AL2" t="s">
         <v>201</v>
       </c>
       <c r="AM2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="AN2" t="s">
         <v>210</v>
@@ -1317,10 +1314,10 @@
         <v>214</v>
       </c>
       <c r="AP2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AQ2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -1370,88 +1367,88 @@
         <v>103</v>
       </c>
       <c r="P3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="Q3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="R3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="S3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="T3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="U3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="V3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="W3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="X3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="Y3" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="Z3" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="AA3" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="AB3" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="AC3" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="AD3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="AE3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="AF3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="AG3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="AH3" t="s">
-        <v>190</v>
+        <v>74</v>
       </c>
       <c r="AI3" t="s">
-        <v>191</v>
+        <v>154</v>
       </c>
       <c r="AJ3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AK3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AL3" t="s">
         <v>202</v>
       </c>
       <c r="AM3" t="s">
-        <v>206</v>
+        <v>74</v>
       </c>
       <c r="AN3" t="s">
         <v>211</v>
       </c>
       <c r="AO3" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="AP3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AQ3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -1498,73 +1495,73 @@
         <v>99</v>
       </c>
       <c r="O4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="P4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Q4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="R4" t="s">
+        <v>119</v>
+      </c>
+      <c r="S4" t="s">
+        <v>124</v>
+      </c>
+      <c r="T4" t="s">
+        <v>129</v>
+      </c>
+      <c r="U4" t="s">
+        <v>134</v>
+      </c>
+      <c r="V4" t="s">
+        <v>139</v>
+      </c>
+      <c r="W4" t="s">
+        <v>144</v>
+      </c>
+      <c r="X4" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>159</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH4" t="s">
         <v>117</v>
       </c>
-      <c r="S4" t="s">
-        <v>98</v>
-      </c>
-      <c r="T4" t="s">
-        <v>79</v>
-      </c>
-      <c r="U4" t="s">
-        <v>130</v>
-      </c>
-      <c r="V4" t="s">
-        <v>135</v>
-      </c>
-      <c r="W4" t="s">
-        <v>140</v>
-      </c>
-      <c r="X4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>149</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>153</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>168</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>172</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>187</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>146</v>
-      </c>
       <c r="AI4" t="s">
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="AJ4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AK4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL4" t="s">
         <v>203</v>
@@ -1576,13 +1573,13 @@
         <v>212</v>
       </c>
       <c r="AO4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AP4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AQ4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -1629,91 +1626,91 @@
         <v>100</v>
       </c>
       <c r="O5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="P5" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="Q5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="R5" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="S5" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="T5" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="U5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="V5" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="W5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="X5" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="Y5" t="s">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="Z5" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="AA5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="AB5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="AC5" t="s">
-        <v>169</v>
+        <v>48</v>
       </c>
       <c r="AD5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AE5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="AF5" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="AG5" t="s">
         <v>188</v>
       </c>
       <c r="AH5" t="s">
-        <v>169</v>
+        <v>73</v>
       </c>
       <c r="AI5" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="AJ5" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="AK5" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="AL5" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="AM5" t="s">
         <v>208</v>
       </c>
       <c r="AN5" t="s">
-        <v>94</v>
+        <v>213</v>
       </c>
       <c r="AO5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AP5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AQ5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -1754,97 +1751,97 @@
         <v>92</v>
       </c>
       <c r="M6" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="N6" t="s">
         <v>101</v>
       </c>
       <c r="O6" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="P6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="Q6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="R6" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="S6" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="T6" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="U6" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="V6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="W6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="X6" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="Y6" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="Z6" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="AA6" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="AB6" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="AC6" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="AD6" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AE6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="AF6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="AG6" t="s">
         <v>189</v>
       </c>
       <c r="AH6" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
       <c r="AI6" t="s">
-        <v>192</v>
+        <v>82</v>
       </c>
       <c r="AJ6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AK6" t="s">
         <v>200</v>
       </c>
       <c r="AL6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="AM6" t="s">
         <v>209</v>
       </c>
       <c r="AN6" t="s">
-        <v>213</v>
+        <v>155</v>
       </c>
       <c r="AO6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AP6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="AQ6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>